<commit_message>
Alterei o background do site
</commit_message>
<xml_diff>
--- a/Projeto-Documentacao/Planilhas/Plano de UAT - Homol 1 Semestre 2019 v1.xlsx
+++ b/Projeto-Documentacao/Planilhas/Plano de UAT - Homol 1 Semestre 2019 v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\grupo3-sa\Projeto-Documentacao\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -410,9 +410,6 @@
     <t>Indicadores de Data e Tempo do Monitoramento por meio de tabelas</t>
   </si>
   <si>
-    <t>Kaio César</t>
-  </si>
-  <si>
     <t>Alerta</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>Após ser feito o cadastro de usuario o usuario pode ter acesso ao sistema</t>
   </si>
   <si>
-    <t xml:space="preserve">deve conter campos de digitação + botão de cadastrar ao sietema e botão de canselar preenchimento de campos  </t>
-  </si>
-  <si>
     <t>RF1.0-02</t>
   </si>
   <si>
@@ -488,10 +482,16 @@
     <t>fazer o armazenamento dos dados importantes</t>
   </si>
   <si>
-    <t xml:space="preserve">campos como nome completo, email, senha e CRF são obrigatorios o preenchimento e devem ser validos </t>
-  </si>
-  <si>
     <t xml:space="preserve">confirmando se os dados são validos, tem acesso ao sistem, caso contrario dois tipos de alerta devem ser emitidos, 1 caso (campos obrigatorios não preenchidos) 2 caso (dados não são validos) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">deve conter campos de digitação + botão de cadastrar ao sistema e botão de canselar preenchimento de campos  </t>
+  </si>
+  <si>
+    <t>Campos como nome completo, email, senha e CRF são obrigatorios o preenchimento e devem ser validos para login de usuário.</t>
+  </si>
+  <si>
+    <t>Caio César</t>
   </si>
 </sst>
 </file>
@@ -1337,6 +1337,109 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1360,74 +1463,17 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1459,52 +1505,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -2021,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53"/>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="105"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="91"/>
       <c r="G2" s="57"/>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
@@ -2075,11 +2075,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="53"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="108"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="94"/>
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -2106,10 +2106,10 @@
       <c r="B5" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="95" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="102"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
       <c r="G5" s="28"/>
@@ -2124,8 +2124,8 @@
       <c r="B6" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="102"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="96"/>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
       <c r="G6" s="28"/>
@@ -2140,8 +2140,8 @@
       <c r="B7" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="102"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="96"/>
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
       <c r="G7" s="28"/>
@@ -2156,8 +2156,8 @@
       <c r="B8" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
       <c r="G8" s="28"/>
@@ -2172,8 +2172,8 @@
       <c r="B9" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="101"/>
-      <c r="D9" s="102"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="96"/>
       <c r="E9" s="28"/>
       <c r="F9" s="29"/>
       <c r="G9" s="28"/>
@@ -2199,16 +2199,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="83"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="113"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="24"/>
@@ -2220,14 +2220,14 @@
       <c r="B12" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="98" t="s">
+      <c r="C12" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="98" t="s">
+      <c r="D12" s="107"/>
+      <c r="E12" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="99"/>
+      <c r="F12" s="107"/>
       <c r="G12" s="72" t="s">
         <v>25</v>
       </c>
@@ -2250,21 +2250,21 @@
       <c r="B13" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="121" t="s">
+      <c r="C13" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="122"/>
-      <c r="E13" s="92" t="s">
+      <c r="D13" s="98"/>
+      <c r="E13" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="100"/>
-      <c r="G13" s="119" t="s">
+      <c r="F13" s="108"/>
+      <c r="G13" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="120">
+      <c r="H13" s="82">
         <v>43608</v>
       </c>
-      <c r="I13" s="119" t="s">
+      <c r="I13" s="81" t="s">
         <v>105</v>
       </c>
       <c r="J13" s="62"/>
@@ -2277,24 +2277,24 @@
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
-      <c r="B14" s="123" t="s">
+      <c r="B14" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="124" t="s">
+      <c r="C14" s="119" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126" t="s">
+      <c r="D14" s="120"/>
+      <c r="E14" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="127"/>
-      <c r="G14" s="128" t="s">
+      <c r="F14" s="110"/>
+      <c r="G14" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="129">
+      <c r="H14" s="85">
         <v>43610</v>
       </c>
-      <c r="I14" s="128" t="s">
+      <c r="I14" s="84" t="s">
         <v>114</v>
       </c>
       <c r="J14" s="62"/>
@@ -2310,21 +2310,21 @@
       <c r="B15" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="121" t="s">
+      <c r="C15" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="122"/>
-      <c r="E15" s="88" t="s">
+      <c r="D15" s="98"/>
+      <c r="E15" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="91"/>
-      <c r="G15" s="119" t="s">
+      <c r="F15" s="99"/>
+      <c r="G15" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="120">
+      <c r="H15" s="82">
         <v>43617</v>
       </c>
-      <c r="I15" s="119" t="s">
+      <c r="I15" s="81" t="s">
         <v>115</v>
       </c>
       <c r="J15" s="62"/>
@@ -2340,21 +2340,21 @@
       <c r="B16" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="97" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="122"/>
-      <c r="E16" s="88" t="s">
+      <c r="D16" s="98"/>
+      <c r="E16" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="119" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" s="120">
+      <c r="F16" s="99"/>
+      <c r="G16" s="81" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" s="82">
         <v>43612</v>
       </c>
-      <c r="I16" s="119" t="s">
+      <c r="I16" s="81" t="s">
         <v>114</v>
       </c>
       <c r="J16" s="62"/>
@@ -2368,23 +2368,23 @@
     <row r="17" spans="1:21" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
       <c r="B17" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="121" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="97" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="98"/>
+      <c r="E17" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="122"/>
-      <c r="E17" s="88" t="s">
+      <c r="F17" s="99"/>
+      <c r="G17" s="81" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="91"/>
-      <c r="G17" s="119" t="s">
-        <v>123</v>
-      </c>
-      <c r="H17" s="120">
+      <c r="H17" s="82">
         <v>43611</v>
       </c>
-      <c r="I17" s="119" t="s">
+      <c r="I17" s="81" t="s">
         <v>115</v>
       </c>
       <c r="J17" s="62"/>
@@ -2415,17 +2415,17 @@
     </row>
     <row r="19" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="55"/>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="115"/>
+      <c r="I19" s="115"/>
+      <c r="J19" s="115"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
     </row>
@@ -2434,18 +2434,18 @@
       <c r="B20" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="94" t="s">
+      <c r="C20" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="94" t="s">
+      <c r="D20" s="103"/>
+      <c r="E20" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="95"/>
-      <c r="G20" s="94" t="s">
+      <c r="F20" s="103"/>
+      <c r="G20" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="95"/>
+      <c r="H20" s="103"/>
       <c r="I20" s="71" t="s">
         <v>27</v>
       </c>
@@ -2462,25 +2462,25 @@
     <row r="21" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="B21" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="87" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="88" t="s">
+      <c r="D21" s="88"/>
+      <c r="E21" s="87" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="88"/>
+      <c r="G21" s="87" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="89"/>
-      <c r="E21" s="88" t="s">
-        <v>141</v>
-      </c>
-      <c r="F21" s="89"/>
-      <c r="G21" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="H21" s="89"/>
+      <c r="H21" s="88"/>
       <c r="I21" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="J21" s="64" t="s">
         <v>131</v>
-      </c>
-      <c r="J21" s="64" t="s">
-        <v>132</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -2492,25 +2492,25 @@
     <row r="22" spans="1:21" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
       <c r="B22" s="63" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="87" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="90"/>
-      <c r="E22" s="92" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="93"/>
-      <c r="G22" s="96" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" s="97"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="100" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="101"/>
+      <c r="G22" s="104" t="s">
+        <v>144</v>
+      </c>
+      <c r="H22" s="105"/>
       <c r="I22" s="66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J22" s="64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K22" s="27"/>
       <c r="L22" s="27"/>
@@ -2522,14 +2522,14 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="54"/>
       <c r="B23" s="63" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="97"/>
+        <v>141</v>
+      </c>
+      <c r="C23" s="87"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="105"/>
       <c r="I23" s="66"/>
       <c r="J23" s="64"/>
       <c r="K23" s="27"/>
@@ -2542,25 +2542,25 @@
     <row r="24" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="54"/>
       <c r="B24" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="88"/>
+      <c r="E24" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="89"/>
-      <c r="E24" s="88" t="s">
-        <v>125</v>
-      </c>
-      <c r="F24" s="89"/>
-      <c r="G24" s="88" t="s">
+      <c r="F24" s="88"/>
+      <c r="G24" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" s="88"/>
+      <c r="I24" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="H24" s="89"/>
-      <c r="I24" s="76" t="s">
+      <c r="J24" s="64" t="s">
         <v>131</v>
-      </c>
-      <c r="J24" s="64" t="s">
-        <v>132</v>
       </c>
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
@@ -2572,25 +2572,25 @@
     <row r="25" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
       <c r="B25" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="80"/>
       <c r="E25" s="73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F25" s="74"/>
       <c r="G25" s="77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H25" s="78"/>
       <c r="I25" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J25" s="64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
@@ -2602,25 +2602,25 @@
     <row r="26" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
       <c r="B26" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="80"/>
       <c r="E26" s="73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" s="74"/>
       <c r="G26" s="77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H26" s="78"/>
       <c r="I26" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J26" s="64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
@@ -2632,12 +2632,12 @@
     <row r="27" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
       <c r="B27" s="63"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="87"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="117"/>
       <c r="I27" s="66"/>
       <c r="J27" s="64"/>
       <c r="K27" s="27"/>
@@ -2684,7 +2684,7 @@
       <c r="B30" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="130">
+      <c r="C30" s="86">
         <v>43598</v>
       </c>
       <c r="D30" s="28"/>
@@ -2783,6 +2783,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="G24:H24"/>
@@ -2799,29 +2822,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I17">
@@ -2952,10 +2952,10 @@
       <c r="A15" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="109"/>
+      <c r="C15" s="121"/>
       <c r="D15" s="41"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3299,20 +3299,20 @@
     <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="122" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="112"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="124"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="113"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="115"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -3507,30 +3507,30 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128"/>
       <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="129" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="117"/>
+      <c r="B24" s="129"/>
       <c r="C24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="12"/>

</xml_diff>

<commit_message>
älterado o insert do node local
</commit_message>
<xml_diff>
--- a/Projeto-Documentacao/Planilhas/Plano de UAT - Homol 1 Semestre 2019 v1.xlsx
+++ b/Projeto-Documentacao/Planilhas/Plano de UAT - Homol 1 Semestre 2019 v1.xlsx
@@ -461,9 +461,6 @@
     <t>Caio César</t>
   </si>
   <si>
-    <t>RF13-2.0</t>
-  </si>
-  <si>
     <t>Os dados do sensor deve ser armazenados em nuvem, tendo assim acesso aos graficos.</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>nome valido e senha valida, direcionar ao sistema caso contrario emitir alerta (nome não encontrado) ou (senha não encontrada)</t>
   </si>
   <si>
-    <t>RF14-2.1</t>
-  </si>
-  <si>
     <t>Graficos deve aparcer e indicar ao usuario taxas tempereturas e umidades</t>
   </si>
   <si>
@@ -500,9 +494,6 @@
     <t>os dados de temperatura e umidade devem ser visualizados pelo usuario diariamente ao acessar o sistema.</t>
   </si>
   <si>
-    <t>RF15-2.2</t>
-  </si>
-  <si>
     <t>Alerta deve ser enviado ao usuario em caso de risco</t>
   </si>
   <si>
@@ -519,6 +510,15 @@
   </si>
   <si>
     <t>RF7-1.1</t>
+  </si>
+  <si>
+    <t>RF10-2.0</t>
+  </si>
+  <si>
+    <t>RF11-2.1</t>
+  </si>
+  <si>
+    <t>RF12-2.2</t>
   </si>
 </sst>
 </file>
@@ -1400,12 +1400,107 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1415,101 +1510,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2059,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2097,13 +2097,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="104"/>
       <c r="G2" s="57"/>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
@@ -2113,11 +2113,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="53"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="95"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="107"/>
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -2144,10 +2144,10 @@
       <c r="B5" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="97"/>
+      <c r="D5" s="98"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
       <c r="G5" s="28"/>
@@ -2162,8 +2162,8 @@
       <c r="B6" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="97"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="98"/>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
       <c r="G6" s="28"/>
@@ -2178,8 +2178,8 @@
       <c r="B7" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
       <c r="G7" s="28"/>
@@ -2194,10 +2194,10 @@
       <c r="B8" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="96" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="97"/>
+      <c r="C8" s="97" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="98"/>
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
       <c r="G8" s="28"/>
@@ -2212,8 +2212,8 @@
       <c r="B9" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="28"/>
       <c r="F9" s="29"/>
       <c r="G9" s="28"/>
@@ -2239,16 +2239,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="108"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="101"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="24"/>
@@ -2260,14 +2260,14 @@
       <c r="B12" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="103"/>
-      <c r="E12" s="102" t="s">
+      <c r="D12" s="83"/>
+      <c r="E12" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="103"/>
+      <c r="F12" s="83"/>
       <c r="G12" s="68" t="s">
         <v>25</v>
       </c>
@@ -2290,14 +2290,14 @@
       <c r="B13" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="98" t="s">
+      <c r="D13" s="92"/>
+      <c r="E13" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="99"/>
+      <c r="F13" s="85"/>
       <c r="G13" s="69" t="s">
         <v>102</v>
       </c>
@@ -2320,14 +2320,14 @@
       <c r="B14" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="112"/>
-      <c r="E14" s="104" t="s">
+      <c r="D14" s="96"/>
+      <c r="E14" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="105"/>
+      <c r="F14" s="91"/>
       <c r="G14" s="72" t="s">
         <v>116</v>
       </c>
@@ -2350,14 +2350,14 @@
       <c r="B15" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="80" t="s">
+      <c r="D15" s="92"/>
+      <c r="E15" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="85"/>
+      <c r="F15" s="92"/>
       <c r="G15" s="69" t="s">
         <v>101</v>
       </c>
@@ -2380,14 +2380,14 @@
       <c r="B16" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="85"/>
-      <c r="E16" s="80" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="85"/>
+      <c r="F16" s="92"/>
       <c r="G16" s="69" t="s">
         <v>136</v>
       </c>
@@ -2410,14 +2410,14 @@
       <c r="B17" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="85"/>
-      <c r="E17" s="80" t="s">
+      <c r="D17" s="92"/>
+      <c r="E17" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="85"/>
+      <c r="F17" s="92"/>
       <c r="G17" s="69" t="s">
         <v>122</v>
       </c>
@@ -2455,17 +2455,17 @@
     </row>
     <row r="19" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="55"/>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
     </row>
@@ -2474,18 +2474,18 @@
       <c r="B20" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="101"/>
-      <c r="E20" s="100" t="s">
+      <c r="D20" s="81"/>
+      <c r="E20" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="G20" s="100" t="s">
+      <c r="F20" s="81"/>
+      <c r="G20" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="101"/>
+      <c r="H20" s="81"/>
       <c r="I20" s="67" t="s">
         <v>27</v>
       </c>
@@ -2502,25 +2502,25 @@
     <row r="21" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="B21" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="80" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="80" t="s">
+      <c r="D21" s="87"/>
+      <c r="E21" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="F21" s="81"/>
-      <c r="G21" s="80" t="s">
+      <c r="F21" s="87"/>
+      <c r="G21" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="81"/>
+      <c r="H21" s="87"/>
       <c r="I21" s="74" t="s">
         <v>126</v>
       </c>
       <c r="J21" s="69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -2532,16 +2532,16 @@
     <row r="22" spans="1:21" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
       <c r="B22" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="80" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="85"/>
-      <c r="E22" s="98" t="s">
+      <c r="D22" s="92"/>
+      <c r="E22" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="F22" s="99"/>
+      <c r="F22" s="85"/>
       <c r="G22" s="88" t="s">
         <v>133</v>
       </c>
@@ -2562,25 +2562,25 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="54"/>
       <c r="B23" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="80" t="s">
+      <c r="D23" s="87"/>
+      <c r="E23" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="81"/>
-      <c r="G23" s="80" t="s">
+      <c r="F23" s="87"/>
+      <c r="G23" s="86" t="s">
         <v>125</v>
       </c>
-      <c r="H23" s="81"/>
+      <c r="H23" s="87"/>
       <c r="I23" s="74" t="s">
         <v>126</v>
       </c>
       <c r="J23" s="69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
@@ -2592,18 +2592,18 @@
     <row r="24" spans="1:21" s="4" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="54"/>
       <c r="B24" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="86" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="92"/>
+      <c r="E24" s="108" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="85"/>
-      <c r="E24" s="86" t="s">
+      <c r="F24" s="109"/>
+      <c r="G24" s="88" t="s">
         <v>141</v>
-      </c>
-      <c r="F24" s="87"/>
-      <c r="G24" s="88" t="s">
-        <v>142</v>
       </c>
       <c r="H24" s="89"/>
       <c r="I24" s="78" t="s">
@@ -2622,25 +2622,25 @@
     <row r="25" spans="1:21" s="4" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
       <c r="B25" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="86" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="87"/>
+      <c r="E25" s="86" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="80" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="F25" s="82"/>
-      <c r="G25" s="83" t="s">
-        <v>147</v>
-      </c>
-      <c r="H25" s="84"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="111" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" s="112"/>
       <c r="I25" s="76" t="s">
         <v>126</v>
       </c>
       <c r="J25" s="69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
@@ -2652,25 +2652,25 @@
     <row r="26" spans="1:21" s="4" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
       <c r="B26" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="80" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="80" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="85"/>
-      <c r="G26" s="83" t="s">
-        <v>149</v>
-      </c>
-      <c r="H26" s="84"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="86" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="92"/>
+      <c r="G26" s="111" t="s">
+        <v>147</v>
+      </c>
+      <c r="H26" s="112"/>
       <c r="I26" s="76" t="s">
         <v>128</v>
       </c>
       <c r="J26" s="69" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
@@ -2682,25 +2682,25 @@
     <row r="27" spans="1:21" s="4" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
       <c r="B27" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="86" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="92"/>
+      <c r="E27" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="85"/>
-      <c r="G27" s="83" t="s">
-        <v>152</v>
-      </c>
-      <c r="H27" s="84"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="111" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="112"/>
       <c r="I27" s="76" t="s">
         <v>126</v>
       </c>
       <c r="J27" s="69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
@@ -2863,6 +2863,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E22:F22"/>
@@ -2879,35 +2908,6 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I17">

</xml_diff>